<commit_message>
Addition of new data
Update
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>Name</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>Curtis Jackson</t>
+  </si>
+  <si>
+    <t>Uzi Vert</t>
   </si>
 </sst>
 </file>
@@ -646,10 +649,18 @@
       <c r="P9" s="3"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+      <c r="A10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="3">
+        <v>1233345</v>
+      </c>
+      <c r="C10" s="4">
+        <v>34003</v>
+      </c>
+      <c r="D10" s="3">
+        <v>23221</v>
+      </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
@@ -1488,7 +1499,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C9F2CC3-B336-4DA5-A24A-90E728F8BF6F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{561DB2C4-94A5-4165-93A9-ED7E5227B482}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://www.boldonjames.com/2008/01/sie/internal/label"/>

</xml_diff>